<commit_message>
Updated Large Format Parts list
Now includes isotemp water bath
</commit_message>
<xml_diff>
--- a/Large Format Thermotaxis Arena/Large Format Thermotaxis Setup Parts List.xlsx
+++ b/Large Format Thermotaxis Arena/Large Format Thermotaxis Setup Parts List.xlsx
@@ -5,15 +5,15 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/astrasb/Box Sync/Lab_Hallem/Astra/Thermotaxis/Thermosensation Setup/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/astrasb/Box Sync/Lab_Hallem/Astra/Thermotaxis/Thermosensation Setup/Large Format Thermotaxis Arena/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CC683CE-185B-EF4C-BBAA-00B68B77C8DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DE105E5-1B31-244D-BF6F-35C881CC6611}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10120" yWindow="460" windowWidth="25600" windowHeight="16060" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4580" yWindow="460" windowWidth="28660" windowHeight="17180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Small-format Thermotaxis Arena" sheetId="1" r:id="rId1"/>
+    <sheet name="Large-format Thermotaxis Arena" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="136">
   <si>
     <t>What is it doing?</t>
   </si>
@@ -436,9 +436,6 @@
     <t>Matlab code for triggering camera acqusition avaliable on Github: https://github.com/HallemLab/Labjack_Camera_Trigger</t>
   </si>
   <si>
-    <t>Metal plate</t>
-  </si>
-  <si>
     <t>Trigger Camera Acquisition</t>
   </si>
   <si>
@@ -449,6 +446,18 @@
   </si>
   <si>
     <t>Misc equipment for mounting camera in the cabinet</t>
+  </si>
+  <si>
+    <t>Metal top plate and reservoir blocks</t>
+  </si>
+  <si>
+    <t>Fisher Scientific</t>
+  </si>
+  <si>
+    <t>Isotemp Refrigetated/Heated Circulating Water Bath (exact version not necessary, just needs to hold temps between 0 and at least 60C)</t>
+  </si>
+  <si>
+    <t>13-874-180</t>
   </si>
 </sst>
 </file>
@@ -653,7 +662,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -852,6 +861,7 @@
     <xf numFmtId="0" fontId="12" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="26">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1216,11 +1226,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I58"/>
+  <dimension ref="A1:I59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B41" sqref="B41:I42"/>
+      <selection pane="bottomLeft" activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1676,7 +1686,7 @@
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
       <c r="E19" s="8" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="F19" s="8"/>
       <c r="G19" s="27"/>
@@ -1797,538 +1807,561 @@
       </c>
       <c r="I25" s="46"/>
     </row>
-    <row r="26" spans="1:9" s="48" customFormat="1" ht="30" customHeight="1">
-      <c r="A26" s="69"/>
-      <c r="B26" s="21"/>
-      <c r="C26" s="21" t="s">
+    <row r="26" spans="1:9">
+      <c r="A26" s="68"/>
+      <c r="B26" s="42"/>
+      <c r="C26" t="s">
+        <v>135</v>
+      </c>
+      <c r="D26" t="s">
+        <v>133</v>
+      </c>
+      <c r="E26" t="s">
+        <v>134</v>
+      </c>
+      <c r="F26" t="s">
+        <v>102</v>
+      </c>
+      <c r="G26" s="70">
+        <v>1900</v>
+      </c>
+      <c r="H26" s="70">
+        <v>1900</v>
+      </c>
+      <c r="I26" s="46"/>
+    </row>
+    <row r="27" spans="1:9" s="48" customFormat="1" ht="30" customHeight="1">
+      <c r="A27" s="69"/>
+      <c r="B27" s="21"/>
+      <c r="C27" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="D26" s="18" t="s">
+      <c r="D27" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="E26" s="47" t="s">
+      <c r="E27" s="47" t="s">
         <v>52</v>
       </c>
-      <c r="F26" s="18">
+      <c r="F27" s="18">
         <v>2</v>
       </c>
-      <c r="G26" s="31">
+      <c r="G27" s="31">
         <v>56.95</v>
       </c>
-      <c r="H26" s="31">
+      <c r="H27" s="31">
         <v>113.9</v>
       </c>
-      <c r="I26" s="19" t="s">
+      <c r="I27" s="19" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="1:9" s="38" customFormat="1" ht="17" thickBot="1">
-      <c r="A27" s="37"/>
-      <c r="G27" s="39"/>
-      <c r="H27" s="39"/>
-    </row>
-    <row r="28" spans="1:9" ht="15" customHeight="1">
-      <c r="A28" s="66" t="s">
+    <row r="28" spans="1:9" s="38" customFormat="1" ht="17" thickBot="1">
+      <c r="A28" s="37"/>
+      <c r="G28" s="39"/>
+      <c r="H28" s="39"/>
+    </row>
+    <row r="29" spans="1:9" ht="15" customHeight="1">
+      <c r="A29" s="66" t="s">
         <v>67</v>
       </c>
-      <c r="B28" s="61" t="s">
+      <c r="B29" s="61" t="s">
         <v>67</v>
       </c>
-      <c r="C28" s="61"/>
-      <c r="D28" s="61"/>
-      <c r="E28" s="61"/>
-      <c r="F28" s="61"/>
-      <c r="G28" s="62"/>
-      <c r="H28" s="62"/>
-      <c r="I28" s="61"/>
-    </row>
-    <row r="29" spans="1:9" ht="68">
-      <c r="A29" s="66"/>
-      <c r="B29" s="8" t="s">
+      <c r="C29" s="61"/>
+      <c r="D29" s="61"/>
+      <c r="E29" s="61"/>
+      <c r="F29" s="61"/>
+      <c r="G29" s="62"/>
+      <c r="H29" s="62"/>
+      <c r="I29" s="61"/>
+    </row>
+    <row r="30" spans="1:9" ht="68">
+      <c r="A30" s="66"/>
+      <c r="B30" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8" t="s">
+      <c r="C30" s="8"/>
+      <c r="D30" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="E29" s="10" t="s">
+      <c r="E30" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="F29" s="8"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="27"/>
-      <c r="I29" s="8" t="s">
+      <c r="F30" s="8"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="8" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="60" customHeight="1">
-      <c r="A30" s="66"/>
-      <c r="B30" s="21"/>
-      <c r="C30" s="21"/>
-      <c r="D30" s="21" t="s">
+    <row r="31" spans="1:9" ht="60" customHeight="1">
+      <c r="A31" s="66"/>
+      <c r="B31" s="21"/>
+      <c r="C31" s="21"/>
+      <c r="D31" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="E30" s="21" t="s">
+      <c r="E31" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="F30" s="21"/>
-      <c r="G30" s="30"/>
-      <c r="H30" s="30"/>
-      <c r="I30" s="21"/>
-    </row>
-    <row r="31" spans="1:9" ht="34">
-      <c r="A31" s="66"/>
-      <c r="B31" s="10"/>
-      <c r="C31" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="D31" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="E31" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="F31" s="10">
-        <v>1</v>
-      </c>
-      <c r="G31" s="24">
-        <v>45.5</v>
-      </c>
-      <c r="H31" s="27">
-        <f t="shared" ref="H31" si="1">G31*F31</f>
-        <v>45.5</v>
-      </c>
-      <c r="I31" s="11" t="s">
-        <v>72</v>
-      </c>
+      <c r="F31" s="21"/>
+      <c r="G31" s="30"/>
+      <c r="H31" s="30"/>
+      <c r="I31" s="21"/>
     </row>
     <row r="32" spans="1:9" ht="34">
       <c r="A32" s="66"/>
-      <c r="C32" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="F32" s="5">
+      <c r="B32" s="10"/>
+      <c r="C32" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="F32" s="10">
         <v>1</v>
       </c>
-      <c r="G32" s="23">
-        <v>389</v>
-      </c>
-      <c r="H32" s="30">
-        <f>G32*F32</f>
-        <v>389</v>
-      </c>
-      <c r="I32" s="6" t="s">
-        <v>98</v>
+      <c r="G32" s="24">
+        <v>45.5</v>
+      </c>
+      <c r="H32" s="27">
+        <f t="shared" ref="H32" si="1">G32*F32</f>
+        <v>45.5</v>
+      </c>
+      <c r="I32" s="11" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="34">
       <c r="A33" s="66"/>
-      <c r="B33" s="10"/>
-      <c r="C33" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="D33" s="10" t="s">
+      <c r="C33" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D33" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E33" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="F33" s="8">
+      <c r="E33" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F33" s="5">
         <v>1</v>
       </c>
-      <c r="G33" s="27">
-        <v>12</v>
-      </c>
-      <c r="H33" s="27">
-        <f t="shared" ref="H33:H36" si="2">G33*F33</f>
-        <v>12</v>
-      </c>
-      <c r="I33" s="8" t="s">
-        <v>99</v>
+      <c r="G33" s="23">
+        <v>389</v>
+      </c>
+      <c r="H33" s="30">
+        <f>G33*F33</f>
+        <v>389</v>
+      </c>
+      <c r="I33" s="6" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="34">
       <c r="A34" s="66"/>
-      <c r="B34" s="18"/>
-      <c r="C34" s="18" t="s">
+      <c r="B34" s="10"/>
+      <c r="C34" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="E34" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="F34" s="8">
+        <v>1</v>
+      </c>
+      <c r="G34" s="27">
+        <v>12</v>
+      </c>
+      <c r="H34" s="27">
+        <f t="shared" ref="H34:H37" si="2">G34*F34</f>
+        <v>12</v>
+      </c>
+      <c r="I34" s="8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="34">
+      <c r="A35" s="66"/>
+      <c r="B35" s="18"/>
+      <c r="C35" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="D34" s="18" t="s">
+      <c r="D35" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="E34" s="18" t="s">
+      <c r="E35" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="F34" s="21">
+      <c r="F35" s="21">
         <v>1</v>
       </c>
-      <c r="G34" s="30">
+      <c r="G35" s="30">
         <v>165</v>
       </c>
-      <c r="H34" s="30">
-        <f>G34*F34</f>
+      <c r="H35" s="30">
+        <f>G35*F35</f>
         <v>165</v>
       </c>
-      <c r="I34" s="21" t="s">
+      <c r="I35" s="21" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="17">
-      <c r="A35" s="66"/>
-      <c r="B35" s="9"/>
-      <c r="C35" s="9" t="s">
+    <row r="36" spans="1:9" ht="17">
+      <c r="A36" s="66"/>
+      <c r="B36" s="9"/>
+      <c r="C36" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="D35" s="10" t="s">
+      <c r="D36" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="E35" s="18" t="s">
+      <c r="E36" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="F35" s="10">
+      <c r="F36" s="10">
         <v>1</v>
       </c>
-      <c r="G35" s="24">
+      <c r="G36" s="24">
         <v>2.82</v>
       </c>
-      <c r="H35" s="27">
+      <c r="H36" s="27">
         <f t="shared" si="2"/>
         <v>2.82</v>
       </c>
-      <c r="I35" s="11" t="s">
+      <c r="I36" s="11" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="17">
-      <c r="A36" s="66"/>
-      <c r="B36" s="20"/>
-      <c r="C36" s="20" t="s">
+    <row r="37" spans="1:9" ht="17">
+      <c r="A37" s="66"/>
+      <c r="B37" s="20"/>
+      <c r="C37" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="D36" s="18" t="s">
+      <c r="D37" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="E36" s="18" t="s">
+      <c r="E37" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="F36" s="18">
+      <c r="F37" s="18">
         <v>1</v>
       </c>
-      <c r="G36" s="31">
+      <c r="G37" s="31">
         <v>2.82</v>
       </c>
-      <c r="H36" s="30">
+      <c r="H37" s="30">
         <f t="shared" si="2"/>
         <v>2.82</v>
       </c>
-      <c r="I36" s="19" t="s">
+      <c r="I37" s="19" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="34">
-      <c r="A37" s="66"/>
-      <c r="B37" s="8"/>
-      <c r="C37" s="8" t="s">
+    <row r="38" spans="1:9" ht="34">
+      <c r="A38" s="66"/>
+      <c r="B38" s="8"/>
+      <c r="C38" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="D37" s="8" t="s">
+      <c r="D38" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="E37" s="8" t="s">
+      <c r="E38" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="F37" s="8">
+      <c r="F38" s="8">
         <v>1</v>
       </c>
-      <c r="G37" s="27">
+      <c r="G38" s="27">
         <v>108</v>
       </c>
-      <c r="H37" s="27">
-        <f>G37*F37</f>
+      <c r="H38" s="27">
+        <f>G38*F38</f>
         <v>108</v>
       </c>
-      <c r="I37" s="8" t="s">
+      <c r="I38" s="8" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="17">
-      <c r="A38" s="66"/>
-      <c r="B38" s="4"/>
-      <c r="C38" s="4"/>
-      <c r="D38" s="4" t="s">
+    <row r="39" spans="1:9" ht="17">
+      <c r="A39" s="66"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="E38" s="4" t="s">
+      <c r="E39" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="F38" s="4">
+      <c r="F39" s="4">
         <v>1</v>
       </c>
-      <c r="G38" s="28">
+      <c r="G39" s="28">
         <v>49</v>
       </c>
-      <c r="H38" s="28">
-        <f>G38*F38</f>
+      <c r="H39" s="28">
+        <f>G39*F39</f>
         <v>49</v>
       </c>
-      <c r="I38" s="4"/>
-    </row>
-    <row r="39" spans="1:9" ht="119">
-      <c r="A39" s="66"/>
-      <c r="B39" s="12"/>
-      <c r="C39" s="12"/>
-      <c r="D39" s="12" t="s">
+      <c r="I39" s="4"/>
+    </row>
+    <row r="40" spans="1:9" ht="119">
+      <c r="A40" s="66"/>
+      <c r="B40" s="12"/>
+      <c r="C40" s="12"/>
+      <c r="D40" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="E39" s="12" t="s">
+      <c r="E40" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="F39" s="12">
+      <c r="F40" s="12">
         <v>1</v>
       </c>
-      <c r="G39" s="12">
+      <c r="G40" s="12">
         <v>140.69</v>
       </c>
-      <c r="H39" s="12">
+      <c r="H40" s="12">
         <v>140.69</v>
       </c>
-      <c r="I39" s="12" t="s">
+      <c r="I40" s="12" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="40" spans="1:9" s="38" customFormat="1" ht="18" thickBot="1">
-      <c r="A40" s="66"/>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="F40" s="1"/>
-      <c r="G40" s="1"/>
-      <c r="H40" s="1"/>
-      <c r="I40" s="1"/>
-    </row>
-    <row r="41" spans="1:9" s="8" customFormat="1" ht="85">
+    <row r="41" spans="1:9" s="38" customFormat="1" ht="18" thickBot="1">
       <c r="A41" s="66"/>
-      <c r="B41" s="12" t="s">
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="C41" s="12"/>
-      <c r="D41" s="12"/>
-      <c r="E41" s="12" t="s">
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+    </row>
+    <row r="42" spans="1:9" s="8" customFormat="1" ht="85">
+      <c r="A42" s="66"/>
+      <c r="B42" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="F41" s="12"/>
-      <c r="G41" s="12"/>
-      <c r="H41" s="12"/>
-      <c r="I41" s="12"/>
-    </row>
-    <row r="42" spans="1:9" s="48" customFormat="1" ht="15" customHeight="1">
-      <c r="A42" s="66"/>
-      <c r="B42" s="48" t="s">
+      <c r="C42" s="12"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="E42" s="48" t="s">
+      <c r="F42" s="12"/>
+      <c r="G42" s="12"/>
+      <c r="H42" s="12"/>
+      <c r="I42" s="12"/>
+    </row>
+    <row r="43" spans="1:9" s="48" customFormat="1" ht="15" customHeight="1">
+      <c r="A43" s="66"/>
+      <c r="B43" s="48" t="s">
+        <v>128</v>
+      </c>
+      <c r="E43" s="48" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="15" customHeight="1" thickBot="1">
-      <c r="A43" s="37"/>
-      <c r="B43" s="38"/>
-      <c r="C43" s="38"/>
-      <c r="D43" s="38"/>
-      <c r="E43" s="38"/>
-      <c r="F43" s="38"/>
-      <c r="G43" s="39"/>
-      <c r="H43" s="39"/>
-      <c r="I43" s="38"/>
-    </row>
-    <row r="44" spans="1:9" ht="22" customHeight="1">
-      <c r="A44" s="63" t="s">
+    <row r="44" spans="1:9" ht="15" customHeight="1" thickBot="1">
+      <c r="A44" s="37"/>
+      <c r="B44" s="38"/>
+      <c r="C44" s="38"/>
+      <c r="D44" s="38"/>
+      <c r="E44" s="38"/>
+      <c r="F44" s="38"/>
+      <c r="G44" s="39"/>
+      <c r="H44" s="39"/>
+      <c r="I44" s="38"/>
+    </row>
+    <row r="45" spans="1:9" ht="22" customHeight="1">
+      <c r="A45" s="63" t="s">
         <v>80</v>
       </c>
-      <c r="B44" s="53" t="s">
+      <c r="B45" s="53" t="s">
         <v>80</v>
       </c>
-      <c r="C44" s="53"/>
-      <c r="D44" s="53"/>
-      <c r="E44" s="53"/>
-      <c r="F44" s="53"/>
-      <c r="G44" s="54"/>
-      <c r="H44" s="54"/>
-      <c r="I44" s="53"/>
-    </row>
-    <row r="45" spans="1:9" ht="15" customHeight="1">
-      <c r="A45" s="64"/>
-      <c r="B45" s="4"/>
-      <c r="C45" s="4"/>
-      <c r="D45" s="5" t="s">
+      <c r="C45" s="53"/>
+      <c r="D45" s="53"/>
+      <c r="E45" s="53"/>
+      <c r="F45" s="53"/>
+      <c r="G45" s="54"/>
+      <c r="H45" s="54"/>
+      <c r="I45" s="53"/>
+    </row>
+    <row r="46" spans="1:9" ht="15" customHeight="1">
+      <c r="A46" s="64"/>
+      <c r="B46" s="4"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="E45" s="4"/>
-      <c r="F45" s="4"/>
-      <c r="G45" s="28"/>
-      <c r="H45" s="28"/>
-      <c r="I45" s="4"/>
-    </row>
-    <row r="46" spans="1:9" ht="17">
-      <c r="A46" s="64"/>
-      <c r="B46" s="8"/>
-      <c r="C46" s="8"/>
-      <c r="D46" s="10" t="s">
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
+      <c r="G46" s="28"/>
+      <c r="H46" s="28"/>
+      <c r="I46" s="4"/>
+    </row>
+    <row r="47" spans="1:9" ht="17">
+      <c r="A47" s="64"/>
+      <c r="B47" s="8"/>
+      <c r="C47" s="8"/>
+      <c r="D47" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="E46" s="8"/>
-      <c r="F46" s="8"/>
-      <c r="G46" s="27"/>
-      <c r="H46" s="27"/>
-      <c r="I46" s="8"/>
-    </row>
-    <row r="47" spans="1:9" ht="34">
-      <c r="A47" s="64"/>
-      <c r="B47" s="4"/>
-      <c r="C47" s="4"/>
-      <c r="D47" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="E47" s="4"/>
-      <c r="F47" s="4"/>
-      <c r="G47" s="28"/>
-      <c r="H47" s="28"/>
-      <c r="I47" s="4"/>
+      <c r="E47" s="8"/>
+      <c r="F47" s="8"/>
+      <c r="G47" s="27"/>
+      <c r="H47" s="27"/>
+      <c r="I47" s="8"/>
     </row>
     <row r="48" spans="1:9" ht="34">
       <c r="A48" s="64"/>
-      <c r="B48" s="10"/>
-      <c r="C48" s="10" t="s">
+      <c r="B48" s="4"/>
+      <c r="C48" s="4"/>
+      <c r="D48" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E48" s="4"/>
+      <c r="F48" s="4"/>
+      <c r="G48" s="28"/>
+      <c r="H48" s="28"/>
+      <c r="I48" s="4"/>
+    </row>
+    <row r="49" spans="1:9" ht="34">
+      <c r="A49" s="64"/>
+      <c r="B49" s="10"/>
+      <c r="C49" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="D48" s="10" t="s">
+      <c r="D49" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E48" s="10" t="s">
+      <c r="E49" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="F48" s="10">
+      <c r="F49" s="10">
         <v>1</v>
       </c>
-      <c r="G48" s="24">
+      <c r="G49" s="24">
         <v>16.920000000000002</v>
       </c>
-      <c r="H48" s="24">
+      <c r="H49" s="24">
         <v>16.920000000000002</v>
       </c>
-      <c r="I48" s="11" t="s">
+      <c r="I49" s="11" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="136">
-      <c r="A49" s="64"/>
-      <c r="B49" s="4"/>
-      <c r="C49" s="4"/>
-      <c r="D49" s="4" t="s">
+    <row r="50" spans="1:9" ht="136">
+      <c r="A50" s="64"/>
+      <c r="B50" s="4"/>
+      <c r="C50" s="4"/>
+      <c r="D50" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="E49" s="50" t="s">
+      <c r="E50" s="50" t="s">
         <v>119</v>
       </c>
-      <c r="F49" s="4" t="s">
+      <c r="F50" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="G49" s="52" t="s">
+      <c r="G50" s="52" t="s">
         <v>121</v>
       </c>
-      <c r="H49" s="28"/>
-      <c r="I49" s="51" t="s">
+      <c r="H50" s="28"/>
+      <c r="I50" s="51" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="34">
-      <c r="A50" s="64"/>
-      <c r="B50" s="8"/>
-      <c r="C50" s="8"/>
-      <c r="D50" s="8" t="s">
+    <row r="51" spans="1:9" ht="34">
+      <c r="A51" s="64"/>
+      <c r="B51" s="8"/>
+      <c r="C51" s="8"/>
+      <c r="D51" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="E50" s="8" t="s">
+      <c r="E51" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="F50" s="8"/>
-      <c r="G50" s="27"/>
-      <c r="H50" s="27"/>
-      <c r="I50" s="8"/>
-    </row>
-    <row r="51" spans="1:9" s="40" customFormat="1" ht="68">
-      <c r="A51" s="64"/>
-      <c r="B51" s="15"/>
-      <c r="C51" s="3"/>
-      <c r="D51" s="4" t="s">
+      <c r="F51" s="8"/>
+      <c r="G51" s="27"/>
+      <c r="H51" s="27"/>
+      <c r="I51" s="8"/>
+    </row>
+    <row r="52" spans="1:9" s="40" customFormat="1" ht="68">
+      <c r="A52" s="64"/>
+      <c r="B52" s="15"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E51" s="4" t="s">
+      <c r="E52" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="F51" s="4">
+      <c r="F52" s="4">
         <v>1</v>
       </c>
-      <c r="G51" s="28">
+      <c r="G52" s="28">
         <v>15.99</v>
       </c>
-      <c r="H51" s="28">
+      <c r="H52" s="28">
         <v>15.99</v>
       </c>
-      <c r="I51" s="6" t="s">
+      <c r="I52" s="6" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="34">
-      <c r="A52" s="64"/>
-      <c r="B52" s="8"/>
-      <c r="C52" s="8"/>
-      <c r="D52" s="8"/>
-      <c r="E52" s="8" t="s">
+    <row r="53" spans="1:9" ht="34">
+      <c r="A53" s="64"/>
+      <c r="B53" s="8"/>
+      <c r="C53" s="8"/>
+      <c r="D53" s="8"/>
+      <c r="E53" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="F52" s="8"/>
-      <c r="G52" s="8"/>
-      <c r="H52" s="8"/>
-      <c r="I52" s="8"/>
-    </row>
-    <row r="53" spans="1:9" ht="17">
-      <c r="A53" s="65"/>
-      <c r="B53" s="40"/>
-      <c r="C53" s="40"/>
-      <c r="D53" s="40"/>
-      <c r="E53" s="40" t="s">
+      <c r="F53" s="8"/>
+      <c r="G53" s="8"/>
+      <c r="H53" s="8"/>
+      <c r="I53" s="8"/>
+    </row>
+    <row r="54" spans="1:9" ht="17">
+      <c r="A54" s="65"/>
+      <c r="B54" s="40"/>
+      <c r="C54" s="40"/>
+      <c r="D54" s="40"/>
+      <c r="E54" s="40" t="s">
         <v>110</v>
       </c>
-      <c r="F53" s="40"/>
-      <c r="G53" s="40"/>
-      <c r="H53" s="40"/>
-      <c r="I53" s="40"/>
-    </row>
-    <row r="58" spans="1:9">
-      <c r="H58" s="29"/>
-      <c r="I58" s="29"/>
+      <c r="F54" s="40"/>
+      <c r="G54" s="40"/>
+      <c r="H54" s="40"/>
+      <c r="I54" s="40"/>
+    </row>
+    <row r="59" spans="1:9">
+      <c r="H59" s="29"/>
+      <c r="I59" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="B44:I44"/>
+    <mergeCell ref="B45:I45"/>
     <mergeCell ref="A2:A19"/>
     <mergeCell ref="B3:I3"/>
     <mergeCell ref="B21:I21"/>
     <mergeCell ref="B2:I2"/>
-    <mergeCell ref="B28:I28"/>
-    <mergeCell ref="A44:A53"/>
-    <mergeCell ref="A28:A42"/>
-    <mergeCell ref="A21:A26"/>
+    <mergeCell ref="B29:I29"/>
+    <mergeCell ref="A45:A54"/>
+    <mergeCell ref="A29:A43"/>
+    <mergeCell ref="A21:A27"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="I4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -2343,14 +2376,14 @@
     <hyperlink ref="I14" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
     <hyperlink ref="I15" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
     <hyperlink ref="I16" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="I26" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="I51" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="I27" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="I52" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
     <hyperlink ref="I17" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
     <hyperlink ref="I18" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="I35" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="I36" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="I36" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="I37" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
     <hyperlink ref="I9" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="I48" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="I49" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
     <hyperlink ref="I23" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
     <hyperlink ref="I22" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
   </hyperlinks>

</xml_diff>